<commit_message>
EM200: 5.1.9.0 General X8" 5.1.4.4
</commit_message>
<xml_diff>
--- a/Software version log.xlsx
+++ b/Software version log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allen\Code\TEMIC_Software_Version_Log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01CEA5D-3017-4346-BFCE-81EF00973F1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B82E2E1C-F0FC-4569-8C26-5927FB0F7EAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{19354D41-4291-4A0A-842F-45F8225187C3}"/>
   </bookViews>
@@ -38,7 +38,7 @@
     <author>Allen</author>
   </authors>
   <commentList>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{B77C80BE-FE60-41E9-9995-B459C4D6E35B}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{0E22B40C-F32A-4001-A5B6-64D8223CD591}">
       <text>
         <r>
           <rPr>
@@ -58,11 +58,14 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Branch: LM_VergeBK</t>
+EM200: develop
+General X8: LM_mergeBK
+MCTW X8: MCTW_VAC
+Previous X8 / X6: LM</t>
         </r>
       </text>
     </comment>
-    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{EF01B194-C9EC-4A29-B7CE-962AE122C764}">
+    <comment ref="A12" authorId="0" shapeId="0" xr:uid="{EF01B194-C9EC-4A29-B7CE-962AE122C764}">
       <text>
         <r>
           <rPr>
@@ -86,7 +89,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{43B18588-6B2E-461E-B59D-E9FE976C7A7D}">
+    <comment ref="A15" authorId="0" shapeId="0" xr:uid="{43B18588-6B2E-461E-B59D-E9FE976C7A7D}">
       <text>
         <r>
           <rPr>
@@ -115,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>5.1.8.1</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -253,6 +256,30 @@
   </si>
   <si>
     <t>for D021, Bella say SW can't open, need rebuild SW for her</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.1.9.0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>D022 (Geckos)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.Integrate UPS function into the SW.
+2.Build D022 for Geckos</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.1.4.4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.update version number.
+2.ResizeMode="NoResize"
+3.WindowStartupLocation="CenterScreen"
+4.update coordinate conversion data after use click apply on the coordinate editor.</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -368,7 +395,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -578,23 +605,64 @@
       <right style="dashed">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+      <bottom style="dashed">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="dashed">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color indexed="64"/>
@@ -613,7 +681,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -626,15 +694,9 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -665,17 +727,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -713,15 +766,6 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -740,10 +784,28 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1074,10 +1136,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F71777C-7F3C-4F46-9C8C-6579ED76EC22}">
-  <dimension ref="A1:BB35"/>
+  <dimension ref="A1:BB37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1089,7 +1151,7 @@
     <col min="5" max="16384" width="7.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" s="16" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:54" s="14" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1102,212 +1164,234 @@
       <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="15"/>
-      <c r="AA1" s="15"/>
-      <c r="AB1" s="15"/>
-      <c r="AC1" s="15"/>
-      <c r="AD1" s="15"/>
-      <c r="AE1" s="15"/>
-      <c r="AF1" s="15"/>
-      <c r="AG1" s="15"/>
-      <c r="AH1" s="15"/>
-      <c r="AI1" s="15"/>
-      <c r="AJ1" s="15"/>
-      <c r="AK1" s="15"/>
-      <c r="AL1" s="15"/>
-      <c r="AM1" s="15"/>
-      <c r="AN1" s="15"/>
-      <c r="AO1" s="15"/>
-      <c r="AP1" s="15"/>
-      <c r="AQ1" s="15"/>
-      <c r="AR1" s="15"/>
-      <c r="AS1" s="15"/>
-      <c r="AT1" s="15"/>
-      <c r="AU1" s="15"/>
-      <c r="AV1" s="15"/>
-      <c r="AW1" s="15"/>
-      <c r="AX1" s="15"/>
-      <c r="AY1" s="15"/>
-      <c r="AZ1" s="15"/>
-      <c r="BA1" s="15"/>
-      <c r="BB1" s="15"/>
-    </row>
-    <row r="2" spans="1:54" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="13"/>
+      <c r="AB1" s="13"/>
+      <c r="AC1" s="13"/>
+      <c r="AD1" s="13"/>
+      <c r="AE1" s="13"/>
+      <c r="AF1" s="13"/>
+      <c r="AG1" s="13"/>
+      <c r="AH1" s="13"/>
+      <c r="AI1" s="13"/>
+      <c r="AJ1" s="13"/>
+      <c r="AK1" s="13"/>
+      <c r="AL1" s="13"/>
+      <c r="AM1" s="13"/>
+      <c r="AN1" s="13"/>
+      <c r="AO1" s="13"/>
+      <c r="AP1" s="13"/>
+      <c r="AQ1" s="13"/>
+      <c r="AR1" s="13"/>
+      <c r="AS1" s="13"/>
+      <c r="AT1" s="13"/>
+      <c r="AU1" s="13"/>
+      <c r="AV1" s="13"/>
+      <c r="AW1" s="13"/>
+      <c r="AX1" s="13"/>
+      <c r="AY1" s="13"/>
+      <c r="AZ1" s="13"/>
+      <c r="BA1" s="13"/>
+      <c r="BB1" s="13"/>
+    </row>
+    <row r="2" spans="1:54" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:54" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="40"/>
+      <c r="B3" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C3" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="43" t="s">
+      <c r="D3" s="38" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:54" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34"/>
-      <c r="B3" s="5" t="s">
+    <row r="4" spans="1:54" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="40"/>
+      <c r="B4" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C4" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D4" s="38" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
-      <c r="B4" s="3" t="s">
+    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A5" s="40"/>
+      <c r="B5" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="17" t="s">
+      <c r="C5" s="36"/>
+      <c r="D5" s="38" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
-      <c r="B5" s="4" t="s">
+    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A6" s="40"/>
+      <c r="B6" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="18" t="s">
+      <c r="C6" s="36"/>
+      <c r="D6" s="38" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="19"/>
-    </row>
-    <row r="7" spans="1:54" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
+    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A7" s="41"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="15"/>
+    </row>
+    <row r="8" spans="1:54" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:54" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="29"/>
+      <c r="B9" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C9" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D9" s="35" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A8" s="37"/>
-      <c r="B8" s="7" t="s">
+    <row r="10" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A10" s="29"/>
+      <c r="B10" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D10" s="16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A9" s="38"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="22"/>
-    </row>
-    <row r="10" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
+    <row r="11" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A11" s="30"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="17"/>
+    </row>
+    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A12" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="D12" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
-      <c r="B11" s="10" t="s">
+    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A13" s="26"/>
+      <c r="B13" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="24" t="s">
+      <c r="C13" s="7"/>
+      <c r="D13" s="19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="25"/>
-    </row>
-    <row r="13" spans="1:54" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="39" t="s">
+    <row r="14" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A14" s="27"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="20"/>
+    </row>
+    <row r="15" spans="1:54" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B15" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C15" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="D15" s="21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
-      <c r="B14" s="13" t="s">
+    <row r="16" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A16" s="32"/>
+      <c r="B16" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C16" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="27" t="s">
+      <c r="D16" s="22" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A15" s="41"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="28"/>
-    </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D35" s="29"/>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="33"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="23"/>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A11"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
EM200: 5.1.10.0 General X8 5.1.4.5
</commit_message>
<xml_diff>
--- a/Software version log.xlsx
+++ b/Software version log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allen\Code\TEMIC_Software_Version_Log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BADCB8-F3A2-4DB7-A290-19C9ECCD86FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693ED456-DF4E-46C5-87C8-EA87504C394F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{19354D41-4291-4A0A-842F-45F8225187C3}"/>
   </bookViews>
@@ -65,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{EF01B194-C9EC-4A29-B7CE-962AE122C764}">
+    <comment ref="A15" authorId="0" shapeId="0" xr:uid="{EF01B194-C9EC-4A29-B7CE-962AE122C764}">
       <text>
         <r>
           <rPr>
@@ -89,7 +89,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A16" authorId="0" shapeId="0" xr:uid="{43B18588-6B2E-461E-B59D-E9FE976C7A7D}">
+    <comment ref="A18" authorId="0" shapeId="0" xr:uid="{43B18588-6B2E-461E-B59D-E9FE976C7A7D}">
       <text>
         <r>
           <rPr>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>5.1.8.1</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -288,6 +288,33 @@
   </si>
   <si>
     <t>for D021 testing</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.1.4.5</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>X8-A103/AIBT</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AIBT
+1.SPG
+2.New GV2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.1.10.0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>D023</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.Integrate USE_SCOTCH_GV2 flag.
+2.Add USE_SCOTCH_GV2 flag for D023</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -403,7 +430,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -677,32 +704,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="dashed">
-        <color indexed="64"/>
-      </left>
-      <right style="dashed">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dashed">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -715,7 +716,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -728,9 +729,6 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -759,9 +757,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -770,9 +765,6 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -791,19 +783,25 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -827,26 +825,26 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1176,10 +1174,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F71777C-7F3C-4F46-9C8C-6579ED76EC22}">
-  <dimension ref="A1:BB38"/>
+  <dimension ref="A1:BB40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1191,7 +1189,7 @@
     <col min="5" max="16384" width="7.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" s="14" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:54" s="13" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1204,246 +1202,270 @@
       <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="13"/>
-      <c r="Z1" s="13"/>
-      <c r="AA1" s="13"/>
-      <c r="AB1" s="13"/>
-      <c r="AC1" s="13"/>
-      <c r="AD1" s="13"/>
-      <c r="AE1" s="13"/>
-      <c r="AF1" s="13"/>
-      <c r="AG1" s="13"/>
-      <c r="AH1" s="13"/>
-      <c r="AI1" s="13"/>
-      <c r="AJ1" s="13"/>
-      <c r="AK1" s="13"/>
-      <c r="AL1" s="13"/>
-      <c r="AM1" s="13"/>
-      <c r="AN1" s="13"/>
-      <c r="AO1" s="13"/>
-      <c r="AP1" s="13"/>
-      <c r="AQ1" s="13"/>
-      <c r="AR1" s="13"/>
-      <c r="AS1" s="13"/>
-      <c r="AT1" s="13"/>
-      <c r="AU1" s="13"/>
-      <c r="AV1" s="13"/>
-      <c r="AW1" s="13"/>
-      <c r="AX1" s="13"/>
-      <c r="AY1" s="13"/>
-      <c r="AZ1" s="13"/>
-      <c r="BA1" s="13"/>
-      <c r="BB1" s="13"/>
-    </row>
-    <row r="2" spans="1:54" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="12"/>
+      <c r="AC1" s="12"/>
+      <c r="AD1" s="12"/>
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="12"/>
+      <c r="AI1" s="12"/>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="12"/>
+      <c r="AL1" s="12"/>
+      <c r="AM1" s="12"/>
+      <c r="AN1" s="12"/>
+      <c r="AO1" s="12"/>
+      <c r="AP1" s="12"/>
+      <c r="AQ1" s="12"/>
+      <c r="AR1" s="12"/>
+      <c r="AS1" s="12"/>
+      <c r="AT1" s="12"/>
+      <c r="AU1" s="12"/>
+      <c r="AV1" s="12"/>
+      <c r="AW1" s="12"/>
+      <c r="AX1" s="12"/>
+      <c r="AY1" s="12"/>
+      <c r="AZ1" s="12"/>
+      <c r="BA1" s="12"/>
+      <c r="BB1" s="12"/>
+    </row>
+    <row r="2" spans="1:54" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="34" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A3" s="35"/>
+      <c r="B3" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C3" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D3" s="23" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:54" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="36"/>
-      <c r="B3" s="27" t="s">
+    <row r="4" spans="1:54" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="35"/>
+      <c r="B4" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="43" t="s">
+      <c r="D4" s="24" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:54" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
-      <c r="B4" s="27" t="s">
+    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A5" s="35"/>
+      <c r="B5" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C5" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D5" s="23" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:54" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="36"/>
-      <c r="B5" s="27" t="s">
+    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A6" s="35"/>
+      <c r="B6" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C6" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D6" s="23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A6" s="36"/>
-      <c r="B6" s="27" t="s">
+    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A7" s="35"/>
+      <c r="B7" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="28" t="s">
+      <c r="C7" s="22"/>
+      <c r="D7" s="23" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A7" s="36"/>
-      <c r="B7" s="27" t="s">
+    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A8" s="35"/>
+      <c r="B8" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="28" t="s">
+      <c r="C8" s="22"/>
+      <c r="D8" s="23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A8" s="37"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="15"/>
-    </row>
-    <row r="9" spans="1:54" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
+    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A9" s="40"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="42"/>
+    </row>
+    <row r="10" spans="1:54" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B10" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:54" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="37"/>
+      <c r="B11" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="41" t="s">
+      <c r="C11" s="4"/>
+      <c r="D11" s="14" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:54" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
-      <c r="B10" s="25" t="s">
+    <row r="12" spans="1:54" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="37"/>
+      <c r="B12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D12" s="14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A11" s="38"/>
-      <c r="B11" s="5" t="s">
+    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A13" s="37"/>
+      <c r="B13" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D13" s="14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A12" s="39"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="17"/>
-    </row>
-    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
+    <row r="14" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A14" s="38"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="15"/>
+    </row>
+    <row r="15" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A15" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B15" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C15" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D15" s="26" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
-      <c r="B14" s="8" t="s">
+    <row r="16" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A16" s="29"/>
+      <c r="B16" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="19" t="s">
+      <c r="C16" s="6"/>
+      <c r="D16" s="16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="20"/>
-    </row>
-    <row r="16" spans="1:54" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="30"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="17"/>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B18" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C18" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="D18" s="18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="33"/>
-      <c r="B17" s="11" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="32"/>
+      <c r="B19" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C19" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D19" s="19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="34"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="23"/>
-    </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D38" s="24"/>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="33"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="20"/>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A2:A9"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[5.1.5.0] General X8 [5.4.5.0] MCTW X8 [5.4.5.0] Previous X8
</commit_message>
<xml_diff>
--- a/Software version log.xlsx
+++ b/Software version log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allen\Code\TEMIC_Software_Version_Log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DCC004-8AFD-417A-AC7B-CF3BDD29A9B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477828BF-E82F-4371-BA55-196EAB7C6C6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11745" yWindow="5460" windowWidth="28800" windowHeight="7905" xr2:uid="{19354D41-4291-4A0A-842F-45F8225187C3}"/>
+    <workbookView xWindow="12645" yWindow="-17775" windowWidth="16200" windowHeight="11505" xr2:uid="{19354D41-4291-4A0A-842F-45F8225187C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,60 +65,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="A16" authorId="0" shapeId="0" xr:uid="{EF01B194-C9EC-4A29-B7CE-962AE122C764}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Allen:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Branch: MCTW_VAC</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A19" authorId="0" shapeId="0" xr:uid="{43B18588-6B2E-461E-B59D-E9FE976C7A7D}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Allen:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Branch: LM</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
   <si>
     <t>5.1.8.1</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -323,6 +275,18 @@
   </si>
   <si>
     <t>Bug fixes:add flag to prevent error.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bug fixes: error caused when there is no recipe flag</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.1.5.0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.4.5.0</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -438,7 +402,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -595,32 +559,6 @@
       <top style="dashed">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dashed">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="dashed">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dashed">
-        <color indexed="64"/>
-      </left>
-      <right style="dashed">
-        <color indexed="64"/>
-      </right>
-      <top style="dashed">
-        <color indexed="64"/>
-      </top>
       <bottom style="dashed">
         <color indexed="64"/>
       </bottom>
@@ -737,7 +675,7 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -746,113 +684,113 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1182,10 +1120,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F71777C-7F3C-4F46-9C8C-6579ED76EC22}">
-  <dimension ref="A1:BB41"/>
+  <dimension ref="A1:BB44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1197,7 +1135,7 @@
     <col min="5" max="16384" width="7.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" s="13" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:54" s="10" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1210,59 +1148,59 @@
       <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12"/>
-      <c r="AA1" s="12"/>
-      <c r="AB1" s="12"/>
-      <c r="AC1" s="12"/>
-      <c r="AD1" s="12"/>
-      <c r="AE1" s="12"/>
-      <c r="AF1" s="12"/>
-      <c r="AG1" s="12"/>
-      <c r="AH1" s="12"/>
-      <c r="AI1" s="12"/>
-      <c r="AJ1" s="12"/>
-      <c r="AK1" s="12"/>
-      <c r="AL1" s="12"/>
-      <c r="AM1" s="12"/>
-      <c r="AN1" s="12"/>
-      <c r="AO1" s="12"/>
-      <c r="AP1" s="12"/>
-      <c r="AQ1" s="12"/>
-      <c r="AR1" s="12"/>
-      <c r="AS1" s="12"/>
-      <c r="AT1" s="12"/>
-      <c r="AU1" s="12"/>
-      <c r="AV1" s="12"/>
-      <c r="AW1" s="12"/>
-      <c r="AX1" s="12"/>
-      <c r="AY1" s="12"/>
-      <c r="AZ1" s="12"/>
-      <c r="BA1" s="12"/>
-      <c r="BB1" s="12"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="9"/>
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="9"/>
+      <c r="AE1" s="9"/>
+      <c r="AF1" s="9"/>
+      <c r="AG1" s="9"/>
+      <c r="AH1" s="9"/>
+      <c r="AI1" s="9"/>
+      <c r="AJ1" s="9"/>
+      <c r="AK1" s="9"/>
+      <c r="AL1" s="9"/>
+      <c r="AM1" s="9"/>
+      <c r="AN1" s="9"/>
+      <c r="AO1" s="9"/>
+      <c r="AP1" s="9"/>
+      <c r="AQ1" s="9"/>
+      <c r="AR1" s="9"/>
+      <c r="AS1" s="9"/>
+      <c r="AT1" s="9"/>
+      <c r="AU1" s="9"/>
+      <c r="AV1" s="9"/>
+      <c r="AW1" s="9"/>
+      <c r="AX1" s="9"/>
+      <c r="AY1" s="9"/>
+      <c r="AZ1" s="9"/>
+      <c r="BA1" s="9"/>
+      <c r="BB1" s="9"/>
     </row>
     <row r="2" spans="1:54" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="31" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1271,222 +1209,255 @@
       <c r="C2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="21" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A3" s="41"/>
-      <c r="B3" s="22" t="s">
+      <c r="A3" s="32"/>
+      <c r="B3" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="17" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:54" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="41"/>
-      <c r="B4" s="22" t="s">
+      <c r="A4" s="32"/>
+      <c r="B4" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="18" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A5" s="41"/>
-      <c r="B5" s="22" t="s">
+      <c r="A5" s="32"/>
+      <c r="B5" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="17" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A6" s="41"/>
-      <c r="B6" s="22" t="s">
+      <c r="A6" s="32"/>
+      <c r="B6" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="17" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A7" s="41"/>
-      <c r="B7" s="22" t="s">
+      <c r="A7" s="32"/>
+      <c r="B7" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="23" t="s">
+      <c r="C7" s="16"/>
+      <c r="D7" s="17" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A8" s="41"/>
-      <c r="B8" s="22" t="s">
+      <c r="A8" s="32"/>
+      <c r="B8" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="23" t="s">
+      <c r="C8" s="16"/>
+      <c r="D8" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A9" s="42"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="31"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="23"/>
     </row>
     <row r="10" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="28" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:54" ht="45" x14ac:dyDescent="0.25">
+      <c r="B10" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="38"/>
       <c r="B11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:54" ht="60" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:54" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="38"/>
       <c r="B12" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:54" ht="45" x14ac:dyDescent="0.25">
+      <c r="D12" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:54" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="38"/>
       <c r="B13" s="4" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:54" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:54" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="38"/>
       <c r="B14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A15" s="38"/>
+      <c r="B15" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D15" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A15" s="39"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="15"/>
-    </row>
     <row r="16" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="39"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="12"/>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B17" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="35"/>
+      <c r="B18" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C18" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D18" s="28" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
-      <c r="B17" s="7" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="35"/>
+      <c r="B19" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="16" t="s">
+      <c r="C19" s="27"/>
+      <c r="D19" s="28" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="33"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="17"/>
-    </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="34" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="36"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="30"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B21" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" s="14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="41"/>
+      <c r="B22" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C22" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D22" s="25" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="35"/>
-      <c r="B20" s="10" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="41"/>
+      <c r="B23" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C23" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D23" s="13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="36"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="20"/>
-    </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D41" s="21"/>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="42"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="14"/>
+    </row>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A19:A21"/>
     <mergeCell ref="A2:A9"/>
-    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="A10:A16"/>
+    <mergeCell ref="A21:A24"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[5.1.10.1] & [5.1.10.0] EM200 [5.1.6.0] General X8
</commit_message>
<xml_diff>
--- a/Software version log.xlsx
+++ b/Software version log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allen\Code\TEMIC_Software_Version_Log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477828BF-E82F-4371-BA55-196EAB7C6C6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854314A0-2D53-4EFE-9EE5-DCF9B6C2826F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12645" yWindow="-17775" windowWidth="16200" windowHeight="11505" xr2:uid="{19354D41-4291-4A0A-842F-45F8225187C3}"/>
+    <workbookView xWindow="3000" yWindow="3000" windowWidth="21600" windowHeight="11505" xr2:uid="{19354D41-4291-4A0A-842F-45F8225187C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="56">
   <si>
     <t>5.1.8.1</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -287,6 +287,26 @@
   </si>
   <si>
     <t>5.4.5.0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>D019</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>For ITRI</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.1.10.1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.1.6.0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCS capture function add 1s delay between off &amp; save image</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -726,9 +746,6 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -756,13 +773,7 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -791,6 +802,15 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1120,10 +1140,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F71777C-7F3C-4F46-9C8C-6579ED76EC22}">
-  <dimension ref="A1:BB44"/>
+  <dimension ref="A1:BB46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1199,261 +1219,285 @@
       <c r="BA1" s="9"/>
       <c r="BB1" s="9"/>
     </row>
-    <row r="2" spans="1:54" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+    <row r="2" spans="1:54" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="40" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:54" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="41"/>
+      <c r="B3" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C3" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D3" s="18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A3" s="32"/>
-      <c r="B3" s="16" t="s">
+    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A4" s="41"/>
+      <c r="B4" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C4" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D4" s="17" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:54" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
-      <c r="B4" s="16" t="s">
+    <row r="5" spans="1:54" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="41"/>
+      <c r="B5" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C5" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D5" s="18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
-      <c r="B5" s="16" t="s">
+    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A6" s="41"/>
+      <c r="B6" s="16" t="s">
         <v>28</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
-      <c r="B6" s="16" t="s">
-        <v>29</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>30</v>
       </c>
       <c r="D6" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A7" s="41"/>
+      <c r="B7" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="17" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
-      <c r="B7" s="16" t="s">
+    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A8" s="41"/>
+      <c r="B8" s="16" t="s">
         <v>0</v>
-      </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
-      <c r="B8" s="16" t="s">
-        <v>1</v>
       </c>
       <c r="C8" s="16"/>
       <c r="D8" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A9" s="41"/>
+      <c r="B9" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="23"/>
-    </row>
-    <row r="10" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="37" t="s">
+    <row r="10" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A10" s="42"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="22"/>
+    </row>
+    <row r="11" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B11" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="35"/>
+      <c r="B12" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="38"/>
-      <c r="B11" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:54" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="38"/>
-      <c r="B12" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="35"/>
+      <c r="B13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:54" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="35"/>
+      <c r="B14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:54" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="38"/>
-      <c r="B13" s="4" t="s">
+    <row r="15" spans="1:54" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="35"/>
+      <c r="B15" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:54" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="38"/>
-      <c r="B14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A15" s="38"/>
-      <c r="B15" s="4" t="s">
-        <v>2</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:54" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="35"/>
+      <c r="B16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="35"/>
+      <c r="B17" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A16" s="39"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="12"/>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="34" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="36"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="12"/>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B19" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="26" t="s">
+      <c r="C19" s="6"/>
+      <c r="D19" s="25" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="35"/>
-      <c r="B18" s="27" t="s">
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="32"/>
+      <c r="B20" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C20" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="28" t="s">
+      <c r="D20" s="27" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
-      <c r="B19" s="27" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="32"/>
+      <c r="B21" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="28" t="s">
+      <c r="C21" s="26"/>
+      <c r="D21" s="27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="36"/>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="30"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="40" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="33"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="29"/>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B23" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="14" t="s">
+      <c r="C23" s="8"/>
+      <c r="D23" s="14" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="41"/>
-      <c r="B22" s="24" t="s">
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="38"/>
+      <c r="B24" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="24" t="s">
+      <c r="C24" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="25" t="s">
+      <c r="D24" s="24" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="41"/>
-      <c r="B23" s="7" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="38"/>
+      <c r="B25" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C25" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D25" s="13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="42"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="14"/>
-    </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D44" s="15"/>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="39"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="14"/>
+    </row>
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D46" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="A10:A16"/>
-    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="A11:A18"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[5.1.8.1]<SP> General X8 [5.4.5.0]<SP> Previous X8 & X6
</commit_message>
<xml_diff>
--- a/Software version log.xlsx
+++ b/Software version log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allen\Code\TEMIC_Software_Version_Log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12DE4F7A-EFB7-4BB8-8013-78C665ACF6F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8CAB9F2-5A85-4A55-A212-12F6F4999C1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{19354D41-4291-4A0A-842F-45F8225187C3}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{19354D41-4291-4A0A-842F-45F8225187C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -67,12 +67,60 @@
         </r>
       </text>
     </comment>
+    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{00CB3CAC-B906-482E-A86C-710F6544B005}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Allen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B29" authorId="0" shapeId="0" xr:uid="{0BAF7110-BE06-4296-9BC4-EDFA4367FCDC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Allen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+task-#391ForPreviousX8&amp;X6</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="68">
   <si>
     <t>5.1.8.1</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -338,6 +386,26 @@
   </si>
   <si>
     <t>For ITRI (rebuild, for verification issue)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.1.8.0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Recipe of side inject, do home at beginning.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>X6-B101</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.4.5.1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Special version for PDMC burn mark case</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -345,7 +413,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -420,6 +488,13 @@
       <family val="2"/>
       <charset val="136"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Microsoft JhengHei Light"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -750,7 +825,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -856,6 +931,30 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -865,24 +964,6 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -896,6 +977,15 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1226,10 +1316,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F71777C-7F3C-4F46-9C8C-6579ED76EC22}">
-  <dimension ref="A1:BB50"/>
+  <dimension ref="A1:BB53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1306,7 +1396,7 @@
       <c r="BB1" s="8"/>
     </row>
     <row r="2" spans="1:54" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="40" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1320,7 +1410,7 @@
       </c>
     </row>
     <row r="3" spans="1:54" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="42"/>
+      <c r="A3" s="41"/>
       <c r="B3" s="15" t="s">
         <v>53</v>
       </c>
@@ -1332,7 +1422,7 @@
       </c>
     </row>
     <row r="4" spans="1:54" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="42"/>
+      <c r="A4" s="41"/>
       <c r="B4" s="15" t="s">
         <v>43</v>
       </c>
@@ -1344,7 +1434,7 @@
       </c>
     </row>
     <row r="5" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A5" s="42"/>
+      <c r="A5" s="41"/>
       <c r="B5" s="15" t="s">
         <v>38</v>
       </c>
@@ -1356,7 +1446,7 @@
       </c>
     </row>
     <row r="6" spans="1:54" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="42"/>
+      <c r="A6" s="41"/>
       <c r="B6" s="15" t="s">
         <v>33</v>
       </c>
@@ -1368,7 +1458,7 @@
       </c>
     </row>
     <row r="7" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A7" s="42"/>
+      <c r="A7" s="41"/>
       <c r="B7" s="15" t="s">
         <v>28</v>
       </c>
@@ -1380,7 +1470,7 @@
       </c>
     </row>
     <row r="8" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A8" s="42"/>
+      <c r="A8" s="41"/>
       <c r="B8" s="15" t="s">
         <v>29</v>
       </c>
@@ -1392,7 +1482,7 @@
       </c>
     </row>
     <row r="9" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A9" s="42"/>
+      <c r="A9" s="41"/>
       <c r="B9" s="15" t="s">
         <v>0</v>
       </c>
@@ -1402,7 +1492,7 @@
       </c>
     </row>
     <row r="10" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A10" s="42"/>
+      <c r="A10" s="41"/>
       <c r="B10" s="15" t="s">
         <v>1</v>
       </c>
@@ -1412,13 +1502,13 @@
       </c>
     </row>
     <row r="11" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A11" s="43"/>
+      <c r="A11" s="42"/>
       <c r="B11" s="20"/>
       <c r="C11" s="20"/>
       <c r="D11" s="21"/>
     </row>
     <row r="12" spans="1:54" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="46" t="s">
         <v>56</v>
       </c>
       <c r="B12" s="25" t="s">
@@ -1432,203 +1522,237 @@
       </c>
     </row>
     <row r="13" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A13" s="45"/>
+      <c r="A13" s="47"/>
       <c r="B13" s="27"/>
       <c r="C13" s="27"/>
       <c r="D13" s="28"/>
     </row>
     <row r="14" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="46" t="s">
+      <c r="A14" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="18" t="s">
+      <c r="B14" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="18" t="s">
-        <v>60</v>
+      <c r="D14" s="53" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="47"/>
-      <c r="B15" s="18" t="s">
-        <v>54</v>
+      <c r="A15" s="49"/>
+      <c r="B15" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="49"/>
+      <c r="B16" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="49"/>
+      <c r="B17" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="19" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="47"/>
-      <c r="B16" s="4" t="s">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="49"/>
+      <c r="B18" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
-      <c r="B17" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
-      <c r="B18" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="49"/>
+      <c r="B19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="49"/>
+      <c r="B20" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
-      <c r="B19" s="4" t="s">
+    <row r="21" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="49"/>
+      <c r="B21" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
-      <c r="B20" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="47"/>
-      <c r="B21" s="4" t="s">
-        <v>2</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D21" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="49"/>
+      <c r="B22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="49"/>
+      <c r="B23" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="48"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="11"/>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="35" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="50"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="11"/>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="B25" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="29"/>
-      <c r="D23" s="30" t="s">
+      <c r="C25" s="29"/>
+      <c r="D25" s="30" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="36"/>
-      <c r="B24" s="31" t="s">
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="44"/>
+      <c r="B26" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="31" t="s">
+      <c r="C26" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="32" t="s">
+      <c r="D26" s="32" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="36"/>
-      <c r="B25" s="31" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="44"/>
+      <c r="B27" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="31"/>
-      <c r="D25" s="32" t="s">
+      <c r="C27" s="31"/>
+      <c r="D27" s="32" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="37"/>
-      <c r="B26" s="33"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="34"/>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="38" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="45"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="34"/>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B29" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="36" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="38"/>
+      <c r="B30" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="13" t="s">
+      <c r="C30" s="7"/>
+      <c r="D30" s="13" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="39"/>
-      <c r="B28" s="22" t="s">
+    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="38"/>
+      <c r="B31" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C31" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D28" s="23" t="s">
+      <c r="D31" s="23" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="39"/>
-      <c r="B29" s="6" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="38"/>
+      <c r="B32" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C32" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D32" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="40"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="13"/>
-    </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D50" s="14"/>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="39"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="13"/>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D53" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="A29:A33"/>
     <mergeCell ref="A2:A11"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A25:A28"/>
     <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A22"/>
+    <mergeCell ref="A14:A24"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[5.1.9.0]<SP> General X8 [5.1.9.1]<SP> General X8 [5.4.5.2]<SP> Previous X8 & X6 [5.4.5.3]<SP> Previous X8 & X6
</commit_message>
<xml_diff>
--- a/Software version log.xlsx
+++ b/Software version log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allen\Code\TEMIC_Software_Version_Log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8CAB9F2-5A85-4A55-A212-12F6F4999C1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83D5360-2BCB-4FCC-B44B-08774B63D6BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{19354D41-4291-4A0A-842F-45F8225187C3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{19354D41-4291-4A0A-842F-45F8225187C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{00CB3CAC-B906-482E-A86C-710F6544B005}">
+    <comment ref="B16" authorId="0" shapeId="0" xr:uid="{00CB3CAC-B906-482E-A86C-710F6544B005}">
       <text>
         <r>
           <rPr>
@@ -91,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B29" authorId="0" shapeId="0" xr:uid="{0BAF7110-BE06-4296-9BC4-EDFA4367FCDC}">
+    <comment ref="B33" authorId="0" shapeId="0" xr:uid="{0BAF7110-BE06-4296-9BC4-EDFA4367FCDC}">
       <text>
         <r>
           <rPr>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="74">
   <si>
     <t>5.1.8.1</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -406,6 +406,30 @@
   </si>
   <si>
     <t>Special version for PDMC burn mark case</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>XYR coordinate conversion table add export xy function #395</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.4.5.2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>For new GV2 (temiceng)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>For new GV2 (hobochen)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.4.5.3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Features required for version 5.1.9.0</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -490,7 +514,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFC00000"/>
       <name val="Microsoft JhengHei Light"/>
       <family val="2"/>
       <charset val="136"/>
@@ -937,6 +961,48 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -944,48 +1010,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1316,10 +1340,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F71777C-7F3C-4F46-9C8C-6579ED76EC22}">
-  <dimension ref="A1:BB53"/>
+  <dimension ref="A1:BB57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1531,228 +1555,276 @@
       <c r="A14" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="51" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="52" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="53" t="s">
-        <v>67</v>
+      <c r="B14" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="49"/>
       <c r="B15" s="5" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="49"/>
-      <c r="B16" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18" t="s">
-        <v>60</v>
+      <c r="B16" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="39" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="49"/>
-      <c r="B17" s="18" t="s">
-        <v>54</v>
+      <c r="B17" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="19" t="s">
-        <v>55</v>
+      <c r="D17" s="11" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="49"/>
-      <c r="B18" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="10" t="s">
-        <v>48</v>
+      <c r="B18" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="49"/>
-      <c r="B19" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B19" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="49"/>
       <c r="B20" s="4" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="49"/>
       <c r="B21" s="4" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="49"/>
       <c r="B22" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>19</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C22" s="4"/>
       <c r="D22" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="49"/>
       <c r="B23" s="4" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D23" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="49"/>
+      <c r="B24" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="49"/>
+      <c r="B25" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="50"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="11"/>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="43" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="50"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="11"/>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="29" t="s">
+      <c r="B27" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="29"/>
-      <c r="D25" s="30" t="s">
+      <c r="C27" s="29"/>
+      <c r="D27" s="30" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="44"/>
-      <c r="B26" s="31" t="s">
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="44"/>
+      <c r="B28" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="31" t="s">
+      <c r="C28" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="32" t="s">
+      <c r="D28" s="32" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="44"/>
-      <c r="B27" s="31" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="44"/>
+      <c r="B29" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="31"/>
-      <c r="D27" s="32" t="s">
+      <c r="C29" s="31"/>
+      <c r="D29" s="32" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="45"/>
-      <c r="B28" s="33"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="34"/>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="37" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="45"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="34"/>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="35" t="s">
+      <c r="B31" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="52"/>
+      <c r="B32" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="52"/>
+      <c r="B33" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="35" t="s">
+      <c r="C33" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="D29" s="36" t="s">
+      <c r="D33" s="36" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="38"/>
-      <c r="B30" s="7" t="s">
+    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="52"/>
+      <c r="B34" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="13" t="s">
+      <c r="C34" s="7"/>
+      <c r="D34" s="13" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="38"/>
-      <c r="B31" s="22" t="s">
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="52"/>
+      <c r="B35" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C31" s="22" t="s">
+      <c r="C35" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D31" s="23" t="s">
+      <c r="D35" s="23" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="38"/>
-      <c r="B32" s="6" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="52"/>
+      <c r="B36" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C36" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D32" s="12" t="s">
+      <c r="D36" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="39"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="13"/>
-    </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D53" s="14"/>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="53"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="13"/>
+    </row>
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D57" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="A31:A37"/>
+    <mergeCell ref="A14:A26"/>
     <mergeCell ref="A2:A11"/>
-    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A27:A30"/>
     <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A24"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[5.1.11.0] EM200 [5.1.12.0] EM200
</commit_message>
<xml_diff>
--- a/Software version log.xlsx
+++ b/Software version log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allen\Code\TEMIC_Software_Version_Log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83D5360-2BCB-4FCC-B44B-08774B63D6BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6B1462-D87E-4253-8A7A-1ABE054142FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{19354D41-4291-4A0A-842F-45F8225187C3}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{19354D41-4291-4A0A-842F-45F8225187C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,42 @@
         </r>
       </text>
     </comment>
-    <comment ref="B16" authorId="0" shapeId="0" xr:uid="{00CB3CAC-B906-482E-A86C-710F6544B005}">
+    <comment ref="C17" authorId="0" shapeId="0" xr:uid="{287E8BA1-3825-4734-B629-AE27CB4D7623}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Allen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+X8-A102/F18B
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>與Tillman確認，已使用次版安裝於X8-A102上</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{00CB3CAC-B906-482E-A86C-710F6544B005}">
       <text>
         <r>
           <rPr>
@@ -91,7 +126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B33" authorId="0" shapeId="0" xr:uid="{0BAF7110-BE06-4296-9BC4-EDFA4367FCDC}">
+    <comment ref="B35" authorId="0" shapeId="0" xr:uid="{0BAF7110-BE06-4296-9BC4-EDFA4367FCDC}">
       <text>
         <r>
           <rPr>
@@ -120,7 +155,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="80">
   <si>
     <t>5.1.8.1</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -430,6 +465,30 @@
   </si>
   <si>
     <t>Features required for version 5.1.9.0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>X8-A107/F21 &amp; X8-A102/F18B</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>VT-BOX troubleshooting</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.1.11.0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.1.12.0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>D002</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Revise D002 configuration: OME_OL stage</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -437,7 +496,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -519,6 +578,13 @@
       <family val="2"/>
       <charset val="136"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -558,7 +624,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -837,6 +903,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -922,15 +1001,6 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -970,6 +1040,24 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -988,28 +1076,19 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1340,17 +1419,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F71777C-7F3C-4F46-9C8C-6579ED76EC22}">
-  <dimension ref="A1:BB57"/>
+  <dimension ref="A1:BB59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="89.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="7.5703125" style="2"/>
   </cols>
@@ -1420,411 +1499,433 @@
       <c r="BB1" s="8"/>
     </row>
     <row r="2" spans="1:54" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="43" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="53" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A3" s="44"/>
+      <c r="B3" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:54" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="44"/>
+      <c r="B4" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C4" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D4" s="16" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:54" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="41"/>
-      <c r="B3" s="15" t="s">
+    <row r="5" spans="1:54" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="44"/>
+      <c r="B5" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C5" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D5" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:54" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="41"/>
-      <c r="B4" s="15" t="s">
+    <row r="6" spans="1:54" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="44"/>
+      <c r="B6" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C6" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D6" s="17" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A5" s="41"/>
-      <c r="B5" s="15" t="s">
+    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A7" s="44"/>
+      <c r="B7" s="15" t="s">
         <v>38</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:54" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="41"/>
-      <c r="B6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A7" s="41"/>
-      <c r="B7" s="15" t="s">
-        <v>28</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>30</v>
       </c>
       <c r="D7" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:54" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="44"/>
+      <c r="B8" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A9" s="44"/>
+      <c r="B9" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="16" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A8" s="41"/>
-      <c r="B8" s="15" t="s">
+    <row r="10" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A10" s="44"/>
+      <c r="B10" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C10" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D10" s="16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
-      <c r="B9" s="15" t="s">
+    <row r="11" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A11" s="44"/>
+      <c r="B11" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16" t="s">
+      <c r="C11" s="15"/>
+      <c r="D11" s="16" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
-      <c r="B10" s="15" t="s">
+    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A12" s="44"/>
+      <c r="B12" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="16" t="s">
+      <c r="C12" s="15"/>
+      <c r="D12" s="16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A11" s="42"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="21"/>
-    </row>
-    <row r="12" spans="1:54" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="46" t="s">
+    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A13" s="45"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="21"/>
+    </row>
+    <row r="14" spans="1:54" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B14" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C14" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D14" s="52" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="28"/>
-    </row>
-    <row r="14" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="48" t="s">
+    <row r="15" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A15" s="49"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="25"/>
+    </row>
+    <row r="16" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B16" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D16" s="11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="49"/>
-      <c r="B15" s="5" t="s">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="41"/>
+      <c r="B17" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C17" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="41"/>
+      <c r="B18" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="49"/>
-      <c r="B16" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="39" t="s">
+      <c r="D18" s="36" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="49"/>
-      <c r="B17" s="5" t="s">
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="41"/>
+      <c r="B19" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="49"/>
-      <c r="B18" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="49"/>
-      <c r="B19" s="18" t="s">
-        <v>54</v>
       </c>
       <c r="C19" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="41"/>
+      <c r="B20" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="41"/>
+      <c r="B21" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="19" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="49"/>
-      <c r="B20" s="4" t="s">
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="41"/>
+      <c r="B22" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="49"/>
-      <c r="B21" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="49"/>
-      <c r="B22" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="41"/>
+      <c r="B23" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="41"/>
+      <c r="B24" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="49"/>
-      <c r="B23" s="4" t="s">
+    <row r="25" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="41"/>
+      <c r="B25" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="49"/>
-      <c r="B24" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="49"/>
-      <c r="B25" s="4" t="s">
-        <v>2</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D25" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="41"/>
+      <c r="B26" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="41"/>
+      <c r="B27" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="50"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="11"/>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="43" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="42"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="11"/>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="29" t="s">
+      <c r="B29" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="29"/>
-      <c r="D27" s="30" t="s">
+      <c r="C29" s="26"/>
+      <c r="D29" s="27" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="44"/>
-      <c r="B28" s="31" t="s">
+    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="47"/>
+      <c r="B30" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="31" t="s">
+      <c r="C30" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="32" t="s">
+      <c r="D30" s="29" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="44"/>
-      <c r="B29" s="31" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="47"/>
+      <c r="B31" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="C29" s="31"/>
-      <c r="D29" s="32" t="s">
+      <c r="C31" s="28"/>
+      <c r="D31" s="29" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="45"/>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="34"/>
-    </row>
-    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="51" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="48"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="31"/>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B33" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C33" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D33" s="13" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="52"/>
-      <c r="B32" s="7" t="s">
+    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="38"/>
+      <c r="B34" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C34" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="D34" s="13" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="52"/>
-      <c r="B33" s="35" t="s">
+    <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="38"/>
+      <c r="B35" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="C33" s="35" t="s">
+      <c r="C35" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="D33" s="36" t="s">
+      <c r="D35" s="33" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="52"/>
-      <c r="B34" s="7" t="s">
+    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="38"/>
+      <c r="B36" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C34" s="7"/>
-      <c r="D34" s="13" t="s">
+      <c r="C36" s="7"/>
+      <c r="D36" s="13" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="52"/>
-      <c r="B35" s="22" t="s">
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="38"/>
+      <c r="B37" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C35" s="22" t="s">
+      <c r="C37" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D35" s="23" t="s">
+      <c r="D37" s="23" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="52"/>
-      <c r="B36" s="6" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="38"/>
+      <c r="B38" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C38" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D36" s="12" t="s">
+      <c r="D38" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="53"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="13"/>
-    </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D57" s="14"/>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="39"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="13"/>
+    </row>
+    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D59" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A31:A37"/>
-    <mergeCell ref="A14:A26"/>
-    <mergeCell ref="A2:A11"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="A33:A39"/>
+    <mergeCell ref="A16:A28"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A14:A15"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[5.4.5.3] X8-B102 (X8 09) [5.1.12.1] EM200 [5.1.12.2] EM200 [5.1.12.3] EM200
</commit_message>
<xml_diff>
--- a/Software version log.xlsx
+++ b/Software version log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allen\Code\TEMIC_Software_Version_Log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6B1462-D87E-4253-8A7A-1ABE054142FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CDB69F7-3B75-436B-99AA-635DF779CB6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{19354D41-4291-4A0A-842F-45F8225187C3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{19354D41-4291-4A0A-842F-45F8225187C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C17" authorId="0" shapeId="0" xr:uid="{287E8BA1-3825-4734-B629-AE27CB4D7623}">
+    <comment ref="C22" authorId="0" shapeId="0" xr:uid="{287E8BA1-3825-4734-B629-AE27CB4D7623}">
       <text>
         <r>
           <rPr>
@@ -102,7 +102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{00CB3CAC-B906-482E-A86C-710F6544B005}">
+    <comment ref="B23" authorId="0" shapeId="0" xr:uid="{00CB3CAC-B906-482E-A86C-710F6544B005}">
       <text>
         <r>
           <rPr>
@@ -126,7 +126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B35" authorId="0" shapeId="0" xr:uid="{0BAF7110-BE06-4296-9BC4-EDFA4367FCDC}">
+    <comment ref="B42" authorId="0" shapeId="0" xr:uid="{0BAF7110-BE06-4296-9BC4-EDFA4367FCDC}">
       <text>
         <r>
           <rPr>
@@ -155,7 +155,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="92">
   <si>
     <t>5.1.8.1</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -489,6 +489,63 @@
   </si>
   <si>
     <t>Revise D002 configuration: OME_OL stage</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Discovery</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>X8-B102 (09)
+※SPG replace PG
+※GV6 (involves firmware)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>X8-B102</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.0.16.8</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Move out version]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Move out version]
+1.Add "X8B102_VER" flag.
+2.Remove Recipe Combo S
+3.Remove "Lam product options" in Recipe T/B &amp; S.
+4.Integrate CCS delay time.
+5.Integrate Import xy/Export XY/Export XYR.
+6.Integrate Coordinate Editor
+7.New X8B102 configuration</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.1.12.1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">For Prosol Corp. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.1.12.2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.1.12.3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>For Prosol Corp, add hybrid mode.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>For Prosol Corp, add new GV2 mode.</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -586,7 +643,7 @@
       <charset val="136"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -623,8 +680,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="23">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -877,30 +946,8 @@
       <right style="dashed">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="dashed">
-        <color auto="1"/>
-      </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="dashed">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -916,6 +963,62 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -928,7 +1031,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1040,6 +1143,51 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1049,47 +1197,41 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1419,10 +1561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F71777C-7F3C-4F46-9C8C-6579ED76EC22}">
-  <dimension ref="A1:BB59"/>
+  <dimension ref="A1:BB66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1498,434 +1640,560 @@
       <c r="BA1" s="8"/>
       <c r="BB1" s="8"/>
     </row>
-    <row r="2" spans="1:54" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
+    <row r="2" spans="1:54" s="9" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="64" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="63"/>
+      <c r="S2" s="63"/>
+      <c r="T2" s="63"/>
+      <c r="U2" s="63"/>
+      <c r="V2" s="63"/>
+      <c r="W2" s="63"/>
+      <c r="X2" s="63"/>
+      <c r="Y2" s="63"/>
+      <c r="Z2" s="63"/>
+      <c r="AA2" s="63"/>
+      <c r="AB2" s="63"/>
+      <c r="AC2" s="63"/>
+      <c r="AD2" s="63"/>
+      <c r="AE2" s="63"/>
+      <c r="AF2" s="63"/>
+      <c r="AG2" s="63"/>
+      <c r="AH2" s="63"/>
+      <c r="AI2" s="63"/>
+      <c r="AJ2" s="63"/>
+      <c r="AK2" s="63"/>
+      <c r="AL2" s="63"/>
+      <c r="AM2" s="63"/>
+      <c r="AN2" s="63"/>
+      <c r="AO2" s="63"/>
+      <c r="AP2" s="63"/>
+      <c r="AQ2" s="63"/>
+      <c r="AR2" s="63"/>
+      <c r="AS2" s="63"/>
+      <c r="AT2" s="63"/>
+      <c r="AU2" s="63"/>
+      <c r="AV2" s="63"/>
+      <c r="AW2" s="63"/>
+      <c r="AX2" s="63"/>
+      <c r="AY2" s="63"/>
+      <c r="AZ2" s="63"/>
+      <c r="BA2" s="63"/>
+      <c r="BB2" s="63"/>
+    </row>
+    <row r="3" spans="1:54" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="65"/>
+      <c r="B3" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:54" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="65"/>
+      <c r="B4" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:54" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="65"/>
+      <c r="B5" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C5" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="53" t="s">
+      <c r="D5" s="17" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A3" s="44"/>
-      <c r="B3" s="15" t="s">
+    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A6" s="65"/>
+      <c r="B6" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16" t="s">
+      <c r="C6" s="15"/>
+      <c r="D6" s="16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:54" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="44"/>
-      <c r="B4" s="15" t="s">
+    <row r="7" spans="1:54" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="65"/>
+      <c r="B7" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C7" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D7" s="16" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:54" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="44"/>
-      <c r="B5" s="15" t="s">
+    <row r="8" spans="1:54" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="65"/>
+      <c r="B8" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C8" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D8" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:54" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
-      <c r="B6" s="15" t="s">
+    <row r="9" spans="1:54" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="65"/>
+      <c r="B9" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C9" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D9" s="17" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
-      <c r="B7" s="15" t="s">
+    <row r="10" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A10" s="65"/>
+      <c r="B10" s="15" t="s">
         <v>38</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:54" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
-      <c r="B8" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
-      <c r="B9" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
-      <c r="B10" s="15" t="s">
-        <v>29</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>30</v>
       </c>
       <c r="D10" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:54" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="65"/>
+      <c r="B11" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A12" s="65"/>
+      <c r="B12" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A13" s="65"/>
+      <c r="B13" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
-      <c r="B11" s="15" t="s">
+    <row r="14" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A14" s="65"/>
+      <c r="B14" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="16" t="s">
+      <c r="C14" s="15"/>
+      <c r="D14" s="16" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A12" s="44"/>
-      <c r="B12" s="15" t="s">
+    <row r="15" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A15" s="65"/>
+      <c r="B15" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="16" t="s">
+      <c r="C15" s="15"/>
+      <c r="D15" s="16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A13" s="45"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="21"/>
-    </row>
-    <row r="14" spans="1:54" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="50" t="s">
+    <row r="16" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A16" s="66"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="21"/>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="51" t="s">
+      <c r="B17" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="51" t="s">
+      <c r="C17" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="D14" s="52" t="s">
+      <c r="D17" s="38" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A15" s="49"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="25"/>
-    </row>
-    <row r="16" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="40" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="62"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="25"/>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="45" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="43"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="45"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B21" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C21" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D21" s="41" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="41"/>
-      <c r="B17" s="5" t="s">
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="56"/>
+      <c r="B22" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C22" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D22" s="11" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="41"/>
-      <c r="B18" s="34" t="s">
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="56"/>
+      <c r="B23" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C23" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="36" t="s">
+      <c r="D23" s="36" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
-      <c r="B19" s="5" t="s">
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="56"/>
+      <c r="B24" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C24" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D24" s="11" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="41"/>
-      <c r="B20" s="18" t="s">
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="56"/>
+      <c r="B25" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18" t="s">
+      <c r="C25" s="18"/>
+      <c r="D25" s="42" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="41"/>
-      <c r="B21" s="18" t="s">
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="56"/>
+      <c r="B26" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C26" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D26" s="19" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="41"/>
-      <c r="B22" s="4" t="s">
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="56"/>
+      <c r="B27" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="10" t="s">
+      <c r="C27" s="4"/>
+      <c r="D27" s="10" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="41"/>
-      <c r="B23" s="4" t="s">
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="56"/>
+      <c r="B28" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C28" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D28" s="10" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="41"/>
-      <c r="B24" s="4" t="s">
+    <row r="29" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="56"/>
+      <c r="B29" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="10" t="s">
+      <c r="C29" s="4"/>
+      <c r="D29" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="41"/>
-      <c r="B25" s="4" t="s">
+    <row r="30" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="56"/>
+      <c r="B30" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C30" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D30" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="41"/>
-      <c r="B26" s="4" t="s">
+    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="56"/>
+      <c r="B31" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D31" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="41"/>
-      <c r="B27" s="4" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="56"/>
+      <c r="B32" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C32" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D32" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="42"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="11"/>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="46" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="57"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="11"/>
+    </row>
+    <row r="34" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A34" s="48" t="s">
+        <v>81</v>
+      </c>
+      <c r="B34" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" s="46" t="s">
+        <v>82</v>
+      </c>
+      <c r="D34" s="47" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="49"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="50"/>
+      <c r="D35" s="51"/>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="26" t="s">
+      <c r="B36" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="26"/>
-      <c r="D29" s="27" t="s">
+      <c r="C36" s="26"/>
+      <c r="D36" s="27" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="47"/>
-      <c r="B30" s="28" t="s">
+    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="59"/>
+      <c r="B37" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="28" t="s">
+      <c r="C37" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="D30" s="29" t="s">
+      <c r="D37" s="29" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="47"/>
-      <c r="B31" s="28" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="59"/>
+      <c r="B38" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="C31" s="28"/>
-      <c r="D31" s="29" t="s">
+      <c r="C38" s="28"/>
+      <c r="D38" s="29" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="48"/>
-      <c r="B32" s="30"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="31"/>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="37" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="60"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="31"/>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B40" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C40" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="D40" s="13" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="38"/>
-      <c r="B34" s="7" t="s">
+    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="53"/>
+      <c r="B41" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C41" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D34" s="13" t="s">
+      <c r="D41" s="13" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="38"/>
-      <c r="B35" s="32" t="s">
+    <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="53"/>
+      <c r="B42" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="32" t="s">
+      <c r="C42" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="D35" s="33" t="s">
+      <c r="D42" s="33" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="38"/>
-      <c r="B36" s="7" t="s">
+    <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="53"/>
+      <c r="B43" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C36" s="7"/>
-      <c r="D36" s="13" t="s">
+      <c r="C43" s="7"/>
+      <c r="D43" s="13" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="38"/>
-      <c r="B37" s="22" t="s">
+    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="53"/>
+      <c r="B44" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C37" s="22" t="s">
+      <c r="C44" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D37" s="23" t="s">
+      <c r="D44" s="23" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="38"/>
-      <c r="B38" s="6" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="53"/>
+      <c r="B45" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C45" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D38" s="12" t="s">
+      <c r="D45" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="39"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="13"/>
-    </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D59" s="14"/>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="54"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="13"/>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D66" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="A33:A39"/>
-    <mergeCell ref="A16:A28"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A40:A46"/>
+    <mergeCell ref="A21:A33"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A2:A16"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[5.1.13.0] EM200 [5.1.13.1] EM200 [5.1.13.2] EM200 [5.4.6.0] X8 B102 (09) [5.4.7.0] X8 B102 (09) [5.4.8.0] X8 B102 (09)
</commit_message>
<xml_diff>
--- a/Software version log.xlsx
+++ b/Software version log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allen\Code\TEMIC_Software_Version_Log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CDB69F7-3B75-436B-99AA-635DF779CB6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230C9188-7672-4D60-9A25-B125DC3BD4F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{19354D41-4291-4A0A-842F-45F8225187C3}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{19354D41-4291-4A0A-842F-45F8225187C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C22" authorId="0" shapeId="0" xr:uid="{287E8BA1-3825-4734-B629-AE27CB4D7623}">
+    <comment ref="C25" authorId="0" shapeId="0" xr:uid="{287E8BA1-3825-4734-B629-AE27CB4D7623}">
       <text>
         <r>
           <rPr>
@@ -102,7 +102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B23" authorId="0" shapeId="0" xr:uid="{00CB3CAC-B906-482E-A86C-710F6544B005}">
+    <comment ref="B26" authorId="0" shapeId="0" xr:uid="{00CB3CAC-B906-482E-A86C-710F6544B005}">
       <text>
         <r>
           <rPr>
@@ -126,7 +126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B42" authorId="0" shapeId="0" xr:uid="{0BAF7110-BE06-4296-9BC4-EDFA4367FCDC}">
+    <comment ref="B48" authorId="0" shapeId="0" xr:uid="{0BAF7110-BE06-4296-9BC4-EDFA4367FCDC}">
       <text>
         <r>
           <rPr>
@@ -155,7 +155,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="107">
   <si>
     <t>5.1.8.1</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -493,12 +493,6 @@
   </si>
   <si>
     <t>Discovery</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>X8-B102 (09)
-※SPG replace PG
-※GV6 (involves firmware)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -548,12 +542,124 @@
     <t>For Prosol Corp, add new GV2 mode.</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>5.1.13.0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.1.13.1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>VT-BOX testing</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>For D001</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.4.6.0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remove security control mechanism. 
+Remove option for autofocus.
+Integrating Recipe EDS:
+  1.Recipe XYR
+  2.Recipe Combo T/B</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.1.13.2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>D007</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>D001</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>D011</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>NTHU</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>X8-B102 (09)
+※SPG replace PG
+※GV6 (involves firmware)
+※Manual focus for recipe plate version</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.4.8.0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.4.7.0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Issue fixed: AF function still activated.
+Root cause </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Wingdings"/>
+        <family val="2"/>
+        <charset val="2"/>
+      </rPr>
+      <t></t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Microsoft JhengHei Light"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t xml:space="preserve"> if no press the button to get the focus value, the AF function will be activated.
+Solutions </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Wingdings"/>
+        <family val="2"/>
+        <charset val="2"/>
+      </rPr>
+      <t></t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Microsoft JhengHei Light"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t xml:space="preserve"> forcefully disable the autofocus function.
+Adds the function to automatically turn off scanning after the recipe process is finished.</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Issue fixed: Failure to save image in recipe mode.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -642,6 +748,12 @@
       <family val="3"/>
       <charset val="136"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Wingdings"/>
+      <family val="2"/>
+      <charset val="2"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -1031,7 +1143,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1149,9 +1261,6 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1176,62 +1285,77 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1561,10 +1685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F71777C-7F3C-4F46-9C8C-6579ED76EC22}">
-  <dimension ref="A1:BB66"/>
+  <dimension ref="A1:BB72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1641,559 +1765,732 @@
       <c r="BB1" s="8"/>
     </row>
     <row r="2" spans="1:54" s="9" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="53" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="49"/>
+      <c r="U2" s="49"/>
+      <c r="V2" s="49"/>
+      <c r="W2" s="49"/>
+      <c r="X2" s="49"/>
+      <c r="Y2" s="49"/>
+      <c r="Z2" s="49"/>
+      <c r="AA2" s="49"/>
+      <c r="AB2" s="49"/>
+      <c r="AC2" s="49"/>
+      <c r="AD2" s="49"/>
+      <c r="AE2" s="49"/>
+      <c r="AF2" s="49"/>
+      <c r="AG2" s="49"/>
+      <c r="AH2" s="49"/>
+      <c r="AI2" s="49"/>
+      <c r="AJ2" s="49"/>
+      <c r="AK2" s="49"/>
+      <c r="AL2" s="49"/>
+      <c r="AM2" s="49"/>
+      <c r="AN2" s="49"/>
+      <c r="AO2" s="49"/>
+      <c r="AP2" s="49"/>
+      <c r="AQ2" s="49"/>
+      <c r="AR2" s="49"/>
+      <c r="AS2" s="49"/>
+      <c r="AT2" s="49"/>
+      <c r="AU2" s="49"/>
+      <c r="AV2" s="49"/>
+      <c r="AW2" s="49"/>
+      <c r="AX2" s="49"/>
+      <c r="AY2" s="49"/>
+      <c r="AZ2" s="49"/>
+      <c r="BA2" s="49"/>
+      <c r="BB2" s="49"/>
+    </row>
+    <row r="3" spans="1:54" s="9" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="54"/>
+      <c r="B3" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="49"/>
+      <c r="R3" s="49"/>
+      <c r="S3" s="49"/>
+      <c r="T3" s="49"/>
+      <c r="U3" s="49"/>
+      <c r="V3" s="49"/>
+      <c r="W3" s="49"/>
+      <c r="X3" s="49"/>
+      <c r="Y3" s="49"/>
+      <c r="Z3" s="49"/>
+      <c r="AA3" s="49"/>
+      <c r="AB3" s="49"/>
+      <c r="AC3" s="49"/>
+      <c r="AD3" s="49"/>
+      <c r="AE3" s="49"/>
+      <c r="AF3" s="49"/>
+      <c r="AG3" s="49"/>
+      <c r="AH3" s="49"/>
+      <c r="AI3" s="49"/>
+      <c r="AJ3" s="49"/>
+      <c r="AK3" s="49"/>
+      <c r="AL3" s="49"/>
+      <c r="AM3" s="49"/>
+      <c r="AN3" s="49"/>
+      <c r="AO3" s="49"/>
+      <c r="AP3" s="49"/>
+      <c r="AQ3" s="49"/>
+      <c r="AR3" s="49"/>
+      <c r="AS3" s="49"/>
+      <c r="AT3" s="49"/>
+      <c r="AU3" s="49"/>
+      <c r="AV3" s="49"/>
+      <c r="AW3" s="49"/>
+      <c r="AX3" s="49"/>
+      <c r="AY3" s="49"/>
+      <c r="AZ3" s="49"/>
+      <c r="BA3" s="49"/>
+      <c r="BB3" s="49"/>
+    </row>
+    <row r="4" spans="1:54" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="54"/>
+      <c r="B4" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:54" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="54"/>
+      <c r="B5" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="49"/>
+      <c r="N5" s="49"/>
+      <c r="O5" s="49"/>
+      <c r="P5" s="49"/>
+      <c r="Q5" s="49"/>
+      <c r="R5" s="49"/>
+      <c r="S5" s="49"/>
+      <c r="T5" s="49"/>
+      <c r="U5" s="49"/>
+      <c r="V5" s="49"/>
+      <c r="W5" s="49"/>
+      <c r="X5" s="49"/>
+      <c r="Y5" s="49"/>
+      <c r="Z5" s="49"/>
+      <c r="AA5" s="49"/>
+      <c r="AB5" s="49"/>
+      <c r="AC5" s="49"/>
+      <c r="AD5" s="49"/>
+      <c r="AE5" s="49"/>
+      <c r="AF5" s="49"/>
+      <c r="AG5" s="49"/>
+      <c r="AH5" s="49"/>
+      <c r="AI5" s="49"/>
+      <c r="AJ5" s="49"/>
+      <c r="AK5" s="49"/>
+      <c r="AL5" s="49"/>
+      <c r="AM5" s="49"/>
+      <c r="AN5" s="49"/>
+      <c r="AO5" s="49"/>
+      <c r="AP5" s="49"/>
+      <c r="AQ5" s="49"/>
+      <c r="AR5" s="49"/>
+      <c r="AS5" s="49"/>
+      <c r="AT5" s="49"/>
+      <c r="AU5" s="49"/>
+      <c r="AV5" s="49"/>
+      <c r="AW5" s="49"/>
+      <c r="AX5" s="49"/>
+      <c r="AY5" s="49"/>
+      <c r="AZ5" s="49"/>
+      <c r="BA5" s="49"/>
+      <c r="BB5" s="49"/>
+    </row>
+    <row r="6" spans="1:54" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="54"/>
+      <c r="B6" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="3" t="s">
+    </row>
+    <row r="7" spans="1:54" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="54"/>
+      <c r="B7" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="39" t="s">
-        <v>91</v>
-      </c>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63"/>
-      <c r="L2" s="63"/>
-      <c r="M2" s="63"/>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63"/>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63"/>
-      <c r="R2" s="63"/>
-      <c r="S2" s="63"/>
-      <c r="T2" s="63"/>
-      <c r="U2" s="63"/>
-      <c r="V2" s="63"/>
-      <c r="W2" s="63"/>
-      <c r="X2" s="63"/>
-      <c r="Y2" s="63"/>
-      <c r="Z2" s="63"/>
-      <c r="AA2" s="63"/>
-      <c r="AB2" s="63"/>
-      <c r="AC2" s="63"/>
-      <c r="AD2" s="63"/>
-      <c r="AE2" s="63"/>
-      <c r="AF2" s="63"/>
-      <c r="AG2" s="63"/>
-      <c r="AH2" s="63"/>
-      <c r="AI2" s="63"/>
-      <c r="AJ2" s="63"/>
-      <c r="AK2" s="63"/>
-      <c r="AL2" s="63"/>
-      <c r="AM2" s="63"/>
-      <c r="AN2" s="63"/>
-      <c r="AO2" s="63"/>
-      <c r="AP2" s="63"/>
-      <c r="AQ2" s="63"/>
-      <c r="AR2" s="63"/>
-      <c r="AS2" s="63"/>
-      <c r="AT2" s="63"/>
-      <c r="AU2" s="63"/>
-      <c r="AV2" s="63"/>
-      <c r="AW2" s="63"/>
-      <c r="AX2" s="63"/>
-      <c r="AY2" s="63"/>
-      <c r="AZ2" s="63"/>
-      <c r="BA2" s="63"/>
-      <c r="BB2" s="63"/>
-    </row>
-    <row r="3" spans="1:54" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="65"/>
-      <c r="B3" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:54" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="65"/>
-      <c r="B4" s="15" t="s">
+      <c r="D7" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:54" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="65"/>
-      <c r="B5" s="15" t="s">
+    </row>
+    <row r="8" spans="1:54" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="54"/>
+      <c r="B8" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C8" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D8" s="17" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A6" s="65"/>
-      <c r="B6" s="15" t="s">
+    <row r="9" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="54"/>
+      <c r="B9" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16" t="s">
+      <c r="C9" s="15"/>
+      <c r="D9" s="16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:54" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="65"/>
-      <c r="B7" s="15" t="s">
+    <row r="10" spans="1:54" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="54"/>
+      <c r="B10" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C10" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D10" s="16" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:54" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="65"/>
-      <c r="B8" s="15" t="s">
+    <row r="11" spans="1:54" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="54"/>
+      <c r="B11" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C11" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D11" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:54" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="65"/>
-      <c r="B9" s="15" t="s">
+    <row r="12" spans="1:54" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="54"/>
+      <c r="B12" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C12" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D12" s="17" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A10" s="65"/>
-      <c r="B10" s="15" t="s">
+    <row r="13" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="54"/>
+      <c r="B13" s="15" t="s">
         <v>38</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:54" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="65"/>
-      <c r="B11" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A12" s="65"/>
-      <c r="B12" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A13" s="65"/>
-      <c r="B13" s="15" t="s">
-        <v>29</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>30</v>
       </c>
       <c r="D13" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:54" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="54"/>
+      <c r="B14" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="54"/>
+      <c r="B15" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="54"/>
+      <c r="B16" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A14" s="65"/>
-      <c r="B14" s="15" t="s">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="54"/>
+      <c r="B17" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="16" t="s">
+      <c r="C17" s="15"/>
+      <c r="D17" s="16" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A15" s="65"/>
-      <c r="B15" s="15" t="s">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="54"/>
+      <c r="B18" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="16" t="s">
+      <c r="C18" s="15"/>
+      <c r="D18" s="16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A16" s="66"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="21"/>
-    </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="61" t="s">
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="55"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="21"/>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="B20" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="37" t="s">
+      <c r="C20" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="38" t="s">
+      <c r="D20" s="38" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="62"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="25"/>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="43" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="66"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="25"/>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="B19" s="44" t="s">
+      <c r="B22" s="43" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="C19" s="44" t="s">
-        <v>80</v>
-      </c>
-      <c r="D19" s="45" t="s">
+    </row>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="42"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="44"/>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="40" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="60"/>
+      <c r="B25" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="60"/>
+      <c r="B26" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="36" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="60"/>
+      <c r="B27" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="60"/>
+      <c r="B28" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="18"/>
+      <c r="D28" s="41" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="60"/>
+      <c r="B29" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="60"/>
+      <c r="B30" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="60"/>
+      <c r="B31" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="60"/>
+      <c r="B32" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" s="4"/>
+      <c r="D32" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A33" s="60"/>
+      <c r="B33" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="60"/>
+      <c r="B34" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="60"/>
+      <c r="B35" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="61"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="11"/>
+    </row>
+    <row r="37" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" s="67" t="s">
+        <v>102</v>
+      </c>
+      <c r="B37" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="C37" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="D37" s="46" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="68"/>
+      <c r="B38" s="51" t="s">
+        <v>104</v>
+      </c>
+      <c r="C38" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="D38" s="70" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="68"/>
+      <c r="B39" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="C39" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="D39" s="52" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A40" s="68"/>
+      <c r="B40" s="51" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="D40" s="52" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="43"/>
-      <c r="B20" s="44"/>
-      <c r="C20" s="44"/>
-      <c r="D20" s="45"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" s="41" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="56"/>
-      <c r="B22" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="56"/>
-      <c r="B23" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="36" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="69"/>
+      <c r="B41" s="47"/>
+      <c r="C41" s="47"/>
+      <c r="D41" s="48"/>
+    </row>
+    <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C42" s="26"/>
+      <c r="D42" s="27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="63"/>
+      <c r="B43" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43" s="29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="63"/>
+      <c r="B44" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" s="28"/>
+      <c r="D44" s="29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="64"/>
+      <c r="B45" s="30"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="31"/>
+    </row>
+    <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="57"/>
+      <c r="B47" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="57"/>
+      <c r="B48" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C48" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="D48" s="33" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="56"/>
-      <c r="B24" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="56"/>
-      <c r="B25" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="42" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="56"/>
-      <c r="B26" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="56"/>
-      <c r="B27" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="10" t="s">
+    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="57"/>
+      <c r="B49" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C49" s="7"/>
+      <c r="D49" s="13" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="56"/>
-      <c r="B28" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="56"/>
-      <c r="B29" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A30" s="56"/>
-      <c r="B30" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="56"/>
-      <c r="B31" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="56"/>
-      <c r="B32" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="57"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="11"/>
-    </row>
-    <row r="34" spans="1:4" ht="120" x14ac:dyDescent="0.25">
-      <c r="A34" s="48" t="s">
-        <v>81</v>
-      </c>
-      <c r="B34" s="46" t="s">
-        <v>72</v>
-      </c>
-      <c r="C34" s="46" t="s">
-        <v>82</v>
-      </c>
-      <c r="D34" s="47" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="49"/>
-      <c r="B35" s="50"/>
-      <c r="C35" s="50"/>
-      <c r="D35" s="51"/>
-    </row>
-    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="58" t="s">
-        <v>12</v>
-      </c>
-      <c r="B36" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="C36" s="26"/>
-      <c r="D36" s="27" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="59"/>
-      <c r="B37" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="D37" s="29" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="59"/>
-      <c r="B38" s="28" t="s">
+    <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="57"/>
+      <c r="B50" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C38" s="28"/>
-      <c r="D38" s="29" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="60"/>
-      <c r="B39" s="30"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="31"/>
-    </row>
-    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="52" t="s">
-        <v>27</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C40" s="7" t="s">
+      <c r="C50" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D50" s="23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="57"/>
+      <c r="B51" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C51" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D40" s="13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="53"/>
-      <c r="B41" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D41" s="13" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="53"/>
-      <c r="B42" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="C42" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="D42" s="33" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="53"/>
-      <c r="B43" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C43" s="7"/>
-      <c r="D43" s="13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="53"/>
-      <c r="B44" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C44" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D44" s="23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="53"/>
-      <c r="B45" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D45" s="12" t="s">
+      <c r="D51" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="54"/>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="13"/>
-    </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D66" s="14"/>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="58"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="13"/>
+    </row>
+    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D72" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A40:A46"/>
-    <mergeCell ref="A21:A33"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A2:A16"/>
+  <mergeCells count="6">
+    <mergeCell ref="A2:A19"/>
+    <mergeCell ref="A46:A52"/>
+    <mergeCell ref="A24:A36"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A37:A41"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[5.1.13.3] EM200 [5.1.13.4] EM200 [5.1.10.1] General X8 [5.4.9.0] X8-B102 Applied
</commit_message>
<xml_diff>
--- a/Software version log.xlsx
+++ b/Software version log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allen\Code\TEMIC_Software_Version_Log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230C9188-7672-4D60-9A25-B125DC3BD4F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6B8463-ABD2-461E-BB02-D06460012AB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{19354D41-4291-4A0A-842F-45F8225187C3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{19354D41-4291-4A0A-842F-45F8225187C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C25" authorId="0" shapeId="0" xr:uid="{287E8BA1-3825-4734-B629-AE27CB4D7623}">
+    <comment ref="C28" authorId="0" shapeId="0" xr:uid="{287E8BA1-3825-4734-B629-AE27CB4D7623}">
       <text>
         <r>
           <rPr>
@@ -102,7 +102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B26" authorId="0" shapeId="0" xr:uid="{00CB3CAC-B906-482E-A86C-710F6544B005}">
+    <comment ref="B29" authorId="0" shapeId="0" xr:uid="{00CB3CAC-B906-482E-A86C-710F6544B005}">
       <text>
         <r>
           <rPr>
@@ -126,7 +126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B48" authorId="0" shapeId="0" xr:uid="{0BAF7110-BE06-4296-9BC4-EDFA4367FCDC}">
+    <comment ref="B52" authorId="0" shapeId="0" xr:uid="{0BAF7110-BE06-4296-9BC4-EDFA4367FCDC}">
       <text>
         <r>
           <rPr>
@@ -155,7 +155,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="114">
   <si>
     <t>5.1.8.1</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -505,17 +505,6 @@
   </si>
   <si>
     <t>[Move out version]</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>[Move out version]
-1.Add "X8B102_VER" flag.
-2.Remove Recipe Combo S
-3.Remove "Lam product options" in Recipe T/B &amp; S.
-4.Integrate CCS delay time.
-5.Integrate Import xy/Export XY/Export XYR.
-6.Integrate Coordinate Editor
-7.New X8B102 configuration</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -652,6 +641,46 @@
   </si>
   <si>
     <t>Issue fixed: Failure to save image in recipe mode.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>X8-B101</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.1.13.3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.1.13.4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>NCKU, add new GV2 mode (X86)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>NCKU, add new GV2 mode (X64)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Move out version]
+1.Add "X8B102_VER" flag.
+2.Remove Recipe Combo S
+3.Remove "Lam product options" in Recipe T/B &amp; S.
+4.Integrate CCS delay time.
+5.Integrate Import xy/Export XY/Export XYR.
+6.Integrate Coordinate Editor
+7.New X8B102 configuration
+8.Issues solved: camera fails to save image when image has no crosshairs.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.4.9.0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Add scale bar insertion option in recipe</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -805,7 +834,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -1077,28 +1106,43 @@
     </border>
     <border>
       <left style="dashed">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="dashed">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
-      <top style="dashed">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="dashed">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="dashed">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1108,9 +1152,7 @@
       <right style="dashed">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -1123,12 +1165,21 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -1143,7 +1194,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1261,23 +1312,14 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1303,14 +1345,50 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1321,15 +1399,6 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1345,17 +1414,20 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1685,10 +1757,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F71777C-7F3C-4F46-9C8C-6579ED76EC22}">
-  <dimension ref="A1:BB72"/>
+  <dimension ref="A1:BB76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1765,732 +1837,878 @@
       <c r="BB1" s="8"/>
     </row>
     <row r="2" spans="1:54" s="9" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="60" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="63" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46"/>
+      <c r="R2" s="46"/>
+      <c r="S2" s="46"/>
+      <c r="T2" s="46"/>
+      <c r="U2" s="46"/>
+      <c r="V2" s="46"/>
+      <c r="W2" s="46"/>
+      <c r="X2" s="46"/>
+      <c r="Y2" s="46"/>
+      <c r="Z2" s="46"/>
+      <c r="AA2" s="46"/>
+      <c r="AB2" s="46"/>
+      <c r="AC2" s="46"/>
+      <c r="AD2" s="46"/>
+      <c r="AE2" s="46"/>
+      <c r="AF2" s="46"/>
+      <c r="AG2" s="46"/>
+      <c r="AH2" s="46"/>
+      <c r="AI2" s="46"/>
+      <c r="AJ2" s="46"/>
+      <c r="AK2" s="46"/>
+      <c r="AL2" s="46"/>
+      <c r="AM2" s="46"/>
+      <c r="AN2" s="46"/>
+      <c r="AO2" s="46"/>
+      <c r="AP2" s="46"/>
+      <c r="AQ2" s="46"/>
+      <c r="AR2" s="46"/>
+      <c r="AS2" s="46"/>
+      <c r="AT2" s="46"/>
+      <c r="AU2" s="46"/>
+      <c r="AV2" s="46"/>
+      <c r="AW2" s="46"/>
+      <c r="AX2" s="46"/>
+      <c r="AY2" s="46"/>
+      <c r="AZ2" s="46"/>
+      <c r="BA2" s="46"/>
+      <c r="BB2" s="46"/>
+    </row>
+    <row r="3" spans="1:54" s="9" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="61"/>
+      <c r="B3" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="64"/>
+      <c r="D3" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="46"/>
+      <c r="P3" s="46"/>
+      <c r="Q3" s="46"/>
+      <c r="R3" s="46"/>
+      <c r="S3" s="46"/>
+      <c r="T3" s="46"/>
+      <c r="U3" s="46"/>
+      <c r="V3" s="46"/>
+      <c r="W3" s="46"/>
+      <c r="X3" s="46"/>
+      <c r="Y3" s="46"/>
+      <c r="Z3" s="46"/>
+      <c r="AA3" s="46"/>
+      <c r="AB3" s="46"/>
+      <c r="AC3" s="46"/>
+      <c r="AD3" s="46"/>
+      <c r="AE3" s="46"/>
+      <c r="AF3" s="46"/>
+      <c r="AG3" s="46"/>
+      <c r="AH3" s="46"/>
+      <c r="AI3" s="46"/>
+      <c r="AJ3" s="46"/>
+      <c r="AK3" s="46"/>
+      <c r="AL3" s="46"/>
+      <c r="AM3" s="46"/>
+      <c r="AN3" s="46"/>
+      <c r="AO3" s="46"/>
+      <c r="AP3" s="46"/>
+      <c r="AQ3" s="46"/>
+      <c r="AR3" s="46"/>
+      <c r="AS3" s="46"/>
+      <c r="AT3" s="46"/>
+      <c r="AU3" s="46"/>
+      <c r="AV3" s="46"/>
+      <c r="AW3" s="46"/>
+      <c r="AX3" s="46"/>
+      <c r="AY3" s="46"/>
+      <c r="AZ3" s="46"/>
+      <c r="BA3" s="46"/>
+      <c r="BB3" s="46"/>
+    </row>
+    <row r="4" spans="1:54" s="9" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="61"/>
+      <c r="B4" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D4" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="46"/>
+      <c r="N4" s="46"/>
+      <c r="O4" s="46"/>
+      <c r="P4" s="46"/>
+      <c r="Q4" s="46"/>
+      <c r="R4" s="46"/>
+      <c r="S4" s="46"/>
+      <c r="T4" s="46"/>
+      <c r="U4" s="46"/>
+      <c r="V4" s="46"/>
+      <c r="W4" s="46"/>
+      <c r="X4" s="46"/>
+      <c r="Y4" s="46"/>
+      <c r="Z4" s="46"/>
+      <c r="AA4" s="46"/>
+      <c r="AB4" s="46"/>
+      <c r="AC4" s="46"/>
+      <c r="AD4" s="46"/>
+      <c r="AE4" s="46"/>
+      <c r="AF4" s="46"/>
+      <c r="AG4" s="46"/>
+      <c r="AH4" s="46"/>
+      <c r="AI4" s="46"/>
+      <c r="AJ4" s="46"/>
+      <c r="AK4" s="46"/>
+      <c r="AL4" s="46"/>
+      <c r="AM4" s="46"/>
+      <c r="AN4" s="46"/>
+      <c r="AO4" s="46"/>
+      <c r="AP4" s="46"/>
+      <c r="AQ4" s="46"/>
+      <c r="AR4" s="46"/>
+      <c r="AS4" s="46"/>
+      <c r="AT4" s="46"/>
+      <c r="AU4" s="46"/>
+      <c r="AV4" s="46"/>
+      <c r="AW4" s="46"/>
+      <c r="AX4" s="46"/>
+      <c r="AY4" s="46"/>
+      <c r="AZ4" s="46"/>
+      <c r="BA4" s="46"/>
+      <c r="BB4" s="46"/>
+    </row>
+    <row r="5" spans="1:54" s="9" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="61"/>
+      <c r="B5" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="50" t="s">
-        <v>101</v>
-      </c>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="49"/>
-      <c r="S2" s="49"/>
-      <c r="T2" s="49"/>
-      <c r="U2" s="49"/>
-      <c r="V2" s="49"/>
-      <c r="W2" s="49"/>
-      <c r="X2" s="49"/>
-      <c r="Y2" s="49"/>
-      <c r="Z2" s="49"/>
-      <c r="AA2" s="49"/>
-      <c r="AB2" s="49"/>
-      <c r="AC2" s="49"/>
-      <c r="AD2" s="49"/>
-      <c r="AE2" s="49"/>
-      <c r="AF2" s="49"/>
-      <c r="AG2" s="49"/>
-      <c r="AH2" s="49"/>
-      <c r="AI2" s="49"/>
-      <c r="AJ2" s="49"/>
-      <c r="AK2" s="49"/>
-      <c r="AL2" s="49"/>
-      <c r="AM2" s="49"/>
-      <c r="AN2" s="49"/>
-      <c r="AO2" s="49"/>
-      <c r="AP2" s="49"/>
-      <c r="AQ2" s="49"/>
-      <c r="AR2" s="49"/>
-      <c r="AS2" s="49"/>
-      <c r="AT2" s="49"/>
-      <c r="AU2" s="49"/>
-      <c r="AV2" s="49"/>
-      <c r="AW2" s="49"/>
-      <c r="AX2" s="49"/>
-      <c r="AY2" s="49"/>
-      <c r="AZ2" s="49"/>
-      <c r="BA2" s="49"/>
-      <c r="BB2" s="49"/>
-    </row>
-    <row r="3" spans="1:54" s="9" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="54"/>
-      <c r="B3" s="15" t="s">
+      <c r="D5" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="46"/>
+      <c r="N5" s="46"/>
+      <c r="O5" s="46"/>
+      <c r="P5" s="46"/>
+      <c r="Q5" s="46"/>
+      <c r="R5" s="46"/>
+      <c r="S5" s="46"/>
+      <c r="T5" s="46"/>
+      <c r="U5" s="46"/>
+      <c r="V5" s="46"/>
+      <c r="W5" s="46"/>
+      <c r="X5" s="46"/>
+      <c r="Y5" s="46"/>
+      <c r="Z5" s="46"/>
+      <c r="AA5" s="46"/>
+      <c r="AB5" s="46"/>
+      <c r="AC5" s="46"/>
+      <c r="AD5" s="46"/>
+      <c r="AE5" s="46"/>
+      <c r="AF5" s="46"/>
+      <c r="AG5" s="46"/>
+      <c r="AH5" s="46"/>
+      <c r="AI5" s="46"/>
+      <c r="AJ5" s="46"/>
+      <c r="AK5" s="46"/>
+      <c r="AL5" s="46"/>
+      <c r="AM5" s="46"/>
+      <c r="AN5" s="46"/>
+      <c r="AO5" s="46"/>
+      <c r="AP5" s="46"/>
+      <c r="AQ5" s="46"/>
+      <c r="AR5" s="46"/>
+      <c r="AS5" s="46"/>
+      <c r="AT5" s="46"/>
+      <c r="AU5" s="46"/>
+      <c r="AV5" s="46"/>
+      <c r="AW5" s="46"/>
+      <c r="AX5" s="46"/>
+      <c r="AY5" s="46"/>
+      <c r="AZ5" s="46"/>
+      <c r="BA5" s="46"/>
+      <c r="BB5" s="46"/>
+    </row>
+    <row r="6" spans="1:54" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="61"/>
+      <c r="B6" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="49"/>
-      <c r="N3" s="49"/>
-      <c r="O3" s="49"/>
-      <c r="P3" s="49"/>
-      <c r="Q3" s="49"/>
-      <c r="R3" s="49"/>
-      <c r="S3" s="49"/>
-      <c r="T3" s="49"/>
-      <c r="U3" s="49"/>
-      <c r="V3" s="49"/>
-      <c r="W3" s="49"/>
-      <c r="X3" s="49"/>
-      <c r="Y3" s="49"/>
-      <c r="Z3" s="49"/>
-      <c r="AA3" s="49"/>
-      <c r="AB3" s="49"/>
-      <c r="AC3" s="49"/>
-      <c r="AD3" s="49"/>
-      <c r="AE3" s="49"/>
-      <c r="AF3" s="49"/>
-      <c r="AG3" s="49"/>
-      <c r="AH3" s="49"/>
-      <c r="AI3" s="49"/>
-      <c r="AJ3" s="49"/>
-      <c r="AK3" s="49"/>
-      <c r="AL3" s="49"/>
-      <c r="AM3" s="49"/>
-      <c r="AN3" s="49"/>
-      <c r="AO3" s="49"/>
-      <c r="AP3" s="49"/>
-      <c r="AQ3" s="49"/>
-      <c r="AR3" s="49"/>
-      <c r="AS3" s="49"/>
-      <c r="AT3" s="49"/>
-      <c r="AU3" s="49"/>
-      <c r="AV3" s="49"/>
-      <c r="AW3" s="49"/>
-      <c r="AX3" s="49"/>
-      <c r="AY3" s="49"/>
-      <c r="AZ3" s="49"/>
-      <c r="BA3" s="49"/>
-      <c r="BB3" s="49"/>
-    </row>
-    <row r="4" spans="1:54" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="54"/>
-      <c r="B4" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="54"/>
-      <c r="B5" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="49"/>
-      <c r="N5" s="49"/>
-      <c r="O5" s="49"/>
-      <c r="P5" s="49"/>
-      <c r="Q5" s="49"/>
-      <c r="R5" s="49"/>
-      <c r="S5" s="49"/>
-      <c r="T5" s="49"/>
-      <c r="U5" s="49"/>
-      <c r="V5" s="49"/>
-      <c r="W5" s="49"/>
-      <c r="X5" s="49"/>
-      <c r="Y5" s="49"/>
-      <c r="Z5" s="49"/>
-      <c r="AA5" s="49"/>
-      <c r="AB5" s="49"/>
-      <c r="AC5" s="49"/>
-      <c r="AD5" s="49"/>
-      <c r="AE5" s="49"/>
-      <c r="AF5" s="49"/>
-      <c r="AG5" s="49"/>
-      <c r="AH5" s="49"/>
-      <c r="AI5" s="49"/>
-      <c r="AJ5" s="49"/>
-      <c r="AK5" s="49"/>
-      <c r="AL5" s="49"/>
-      <c r="AM5" s="49"/>
-      <c r="AN5" s="49"/>
-      <c r="AO5" s="49"/>
-      <c r="AP5" s="49"/>
-      <c r="AQ5" s="49"/>
-      <c r="AR5" s="49"/>
-      <c r="AS5" s="49"/>
-      <c r="AT5" s="49"/>
-      <c r="AU5" s="49"/>
-      <c r="AV5" s="49"/>
-      <c r="AW5" s="49"/>
-      <c r="AX5" s="49"/>
-      <c r="AY5" s="49"/>
-      <c r="AZ5" s="49"/>
-      <c r="BA5" s="49"/>
-      <c r="BB5" s="49"/>
-    </row>
-    <row r="6" spans="1:54" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="54"/>
-      <c r="B6" s="15" t="s">
+    </row>
+    <row r="7" spans="1:54" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="61"/>
+      <c r="B7" s="15" t="s">
         <v>87</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:54" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="54"/>
-      <c r="B7" s="15" t="s">
-        <v>85</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>30</v>
       </c>
       <c r="D7" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="46"/>
+      <c r="N7" s="46"/>
+      <c r="O7" s="46"/>
+      <c r="P7" s="46"/>
+      <c r="Q7" s="46"/>
+      <c r="R7" s="46"/>
+      <c r="S7" s="46"/>
+      <c r="T7" s="46"/>
+      <c r="U7" s="46"/>
+      <c r="V7" s="46"/>
+      <c r="W7" s="46"/>
+      <c r="X7" s="46"/>
+      <c r="Y7" s="46"/>
+      <c r="Z7" s="46"/>
+      <c r="AA7" s="46"/>
+      <c r="AB7" s="46"/>
+      <c r="AC7" s="46"/>
+      <c r="AD7" s="46"/>
+      <c r="AE7" s="46"/>
+      <c r="AF7" s="46"/>
+      <c r="AG7" s="46"/>
+      <c r="AH7" s="46"/>
+      <c r="AI7" s="46"/>
+      <c r="AJ7" s="46"/>
+      <c r="AK7" s="46"/>
+      <c r="AL7" s="46"/>
+      <c r="AM7" s="46"/>
+      <c r="AN7" s="46"/>
+      <c r="AO7" s="46"/>
+      <c r="AP7" s="46"/>
+      <c r="AQ7" s="46"/>
+      <c r="AR7" s="46"/>
+      <c r="AS7" s="46"/>
+      <c r="AT7" s="46"/>
+      <c r="AU7" s="46"/>
+      <c r="AV7" s="46"/>
+      <c r="AW7" s="46"/>
+      <c r="AX7" s="46"/>
+      <c r="AY7" s="46"/>
+      <c r="AZ7" s="46"/>
+      <c r="BA7" s="46"/>
+      <c r="BB7" s="46"/>
+    </row>
+    <row r="8" spans="1:54" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="61"/>
+      <c r="B8" s="15" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="8" spans="1:54" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="54"/>
-      <c r="B8" s="15" t="s">
+      <c r="C8" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:54" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="61"/>
+      <c r="B9" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:54" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="61"/>
+      <c r="B10" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C10" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D10" s="17" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="54"/>
-      <c r="B9" s="15" t="s">
+    <row r="11" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="61"/>
+      <c r="B11" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16" t="s">
+      <c r="C11" s="15"/>
+      <c r="D11" s="16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:54" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="54"/>
-      <c r="B10" s="15" t="s">
+    <row r="12" spans="1:54" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="61"/>
+      <c r="B12" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C12" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D12" s="16" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:54" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="54"/>
-      <c r="B11" s="15" t="s">
+    <row r="13" spans="1:54" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="61"/>
+      <c r="B13" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C13" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D13" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:54" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="54"/>
-      <c r="B12" s="15" t="s">
+    <row r="14" spans="1:54" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="61"/>
+      <c r="B14" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C14" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D14" s="17" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="54"/>
-      <c r="B13" s="15" t="s">
+    <row r="15" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="61"/>
+      <c r="B15" s="15" t="s">
         <v>38</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:54" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="54"/>
-      <c r="B14" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="54"/>
-      <c r="B15" s="15" t="s">
-        <v>28</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>30</v>
       </c>
       <c r="D15" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:54" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="61"/>
+      <c r="B16" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="61"/>
+      <c r="B17" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="16" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="54"/>
-      <c r="B16" s="15" t="s">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="61"/>
+      <c r="B18" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C18" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D18" s="16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="54"/>
-      <c r="B17" s="15" t="s">
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="61"/>
+      <c r="B19" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="16" t="s">
+      <c r="C19" s="15"/>
+      <c r="D19" s="16" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="54"/>
-      <c r="B18" s="15" t="s">
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="61"/>
+      <c r="B20" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="16" t="s">
+      <c r="C20" s="15"/>
+      <c r="D20" s="16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="55"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="21"/>
-    </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="65" t="s">
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="62"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="21"/>
+    </row>
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="71" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="37" t="s">
+      <c r="B22" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="37" t="s">
+      <c r="C22" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="38" t="s">
+      <c r="D22" s="38" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="66"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="25"/>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="42" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="72"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="25"/>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="B22" s="43" t="s">
+      <c r="B24" s="54" t="s">
         <v>82</v>
       </c>
-      <c r="C22" s="43" t="s">
+      <c r="C24" s="54" t="s">
         <v>80</v>
       </c>
-      <c r="D22" s="44" t="s">
+      <c r="D24" s="55" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="42"/>
-      <c r="B23" s="43"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="44"/>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="59" t="s">
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="59"/>
+      <c r="B25" s="56"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="57"/>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="39" t="s">
+      <c r="B26" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="52" t="s">
+        <v>106</v>
+      </c>
+      <c r="D26" s="53"/>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="73"/>
+      <c r="B27" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C27" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="40" t="s">
+      <c r="D27" s="40" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="60"/>
-      <c r="B25" s="5" t="s">
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="73"/>
+      <c r="B28" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C28" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D28" s="11" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="60"/>
-      <c r="B26" s="34" t="s">
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="73"/>
+      <c r="B29" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C26" s="35" t="s">
+      <c r="C29" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="36" t="s">
+      <c r="D29" s="36" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="60"/>
-      <c r="B27" s="5" t="s">
+    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="73"/>
+      <c r="B30" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C30" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D30" s="11" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="60"/>
-      <c r="B28" s="18" t="s">
+    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="73"/>
+      <c r="B31" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="41" t="s">
+      <c r="C31" s="18"/>
+      <c r="D31" s="41" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="60"/>
-      <c r="B29" s="18" t="s">
+    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="73"/>
+      <c r="B32" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C32" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D29" s="19" t="s">
+      <c r="D32" s="19" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="60"/>
-      <c r="B30" s="4" t="s">
+    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="73"/>
+      <c r="B33" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="10" t="s">
+      <c r="C33" s="4"/>
+      <c r="D33" s="10" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="60"/>
-      <c r="B31" s="4" t="s">
+    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="73"/>
+      <c r="B34" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C34" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D34" s="10" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="60"/>
-      <c r="B32" s="4" t="s">
+    <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="73"/>
+      <c r="B35" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="10" t="s">
+      <c r="C35" s="4"/>
+      <c r="D35" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A33" s="60"/>
-      <c r="B33" s="4" t="s">
+    <row r="36" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" s="73"/>
+      <c r="B36" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C36" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D36" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="60"/>
-      <c r="B34" s="4" t="s">
+    <row r="37" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="73"/>
+      <c r="B37" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C37" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D37" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="60"/>
-      <c r="B35" s="4" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="73"/>
+      <c r="B38" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C38" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="D38" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="61"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="11"/>
-    </row>
-    <row r="37" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A37" s="67" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="74"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="11"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="75" t="s">
+        <v>101</v>
+      </c>
+      <c r="B40" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="C40" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="D40" s="43" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="76"/>
+      <c r="B41" s="42" t="s">
         <v>102</v>
       </c>
-      <c r="B37" s="45" t="s">
+      <c r="C41" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="D41" s="43" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="76"/>
+      <c r="B42" s="48" t="s">
         <v>103</v>
       </c>
-      <c r="C37" s="45" t="s">
+      <c r="C42" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="D37" s="46" t="s">
+      <c r="D42" s="50" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="68"/>
-      <c r="B38" s="51" t="s">
-        <v>104</v>
-      </c>
-      <c r="C38" s="51" t="s">
+    <row r="43" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="76"/>
+      <c r="B43" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="C43" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="D38" s="70" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="68"/>
-      <c r="B39" s="51" t="s">
+      <c r="D43" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="C39" s="51" t="s">
+    </row>
+    <row r="44" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A44" s="76"/>
+      <c r="B44" s="48" t="s">
+        <v>72</v>
+      </c>
+      <c r="C44" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="D39" s="52" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="120" x14ac:dyDescent="0.25">
-      <c r="A40" s="68"/>
-      <c r="B40" s="51" t="s">
+      <c r="D44" s="49" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="77"/>
+      <c r="B45" s="44"/>
+      <c r="C45" s="44"/>
+      <c r="D45" s="45"/>
+    </row>
+    <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="68" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C46" s="26"/>
+      <c r="D46" s="27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="69"/>
+      <c r="B47" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="D47" s="29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="69"/>
+      <c r="B48" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" s="28"/>
+      <c r="D48" s="29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="70"/>
+      <c r="B49" s="30"/>
+      <c r="C49" s="30"/>
+      <c r="D49" s="31"/>
+    </row>
+    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="B50" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C40" s="51" t="s">
-        <v>81</v>
-      </c>
-      <c r="D40" s="52" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="69"/>
-      <c r="B41" s="47"/>
-      <c r="C41" s="47"/>
-      <c r="D41" s="48"/>
-    </row>
-    <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="B42" s="26" t="s">
+      <c r="C50" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="66"/>
+      <c r="B51" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D51" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="66"/>
+      <c r="B52" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C52" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="D52" s="33" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="66"/>
+      <c r="B53" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C42" s="26"/>
-      <c r="D42" s="27" t="s">
+      <c r="C53" s="7"/>
+      <c r="D53" s="13" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="63"/>
-      <c r="B43" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C43" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="D43" s="29" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="63"/>
-      <c r="B44" s="28" t="s">
+    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="66"/>
+      <c r="B54" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C44" s="28"/>
-      <c r="D44" s="29" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="64"/>
-      <c r="B45" s="30"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="31"/>
-    </row>
-    <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C46" s="7" t="s">
+      <c r="C54" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D54" s="23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="66"/>
+      <c r="B55" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C55" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D46" s="13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="57"/>
-      <c r="B47" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D47" s="13" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="57"/>
-      <c r="B48" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="C48" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="D48" s="33" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="57"/>
-      <c r="B49" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C49" s="7"/>
-      <c r="D49" s="13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="57"/>
-      <c r="B50" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C50" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D50" s="23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="57"/>
-      <c r="B51" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D51" s="12" t="s">
+      <c r="D55" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="58"/>
-      <c r="B52" s="7"/>
-      <c r="C52" s="7"/>
-      <c r="D52" s="13"/>
-    </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D72" s="14"/>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="67"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="13"/>
+    </row>
+    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D76" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A2:A19"/>
-    <mergeCell ref="A46:A52"/>
-    <mergeCell ref="A24:A36"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A37:A41"/>
+  <mergeCells count="8">
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A2:A21"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="A50:A56"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A26:A39"/>
+    <mergeCell ref="A40:A45"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>